<commit_message>
Signup Mortigate and Login  Api's  commited By 'Lakshmi'
</commit_message>
<xml_diff>
--- a/Mortgage_Data_Contract.xlsx
+++ b/Mortgage_Data_Contract.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -83,24 +83,11 @@
   </si>
   <si>
     <t>varchar</t>
-  </si>
-  <si>
-    <t>{
-adminId: Long
-}</t>
   </si>
   <si>
     <t>{
 userId: Long,password: String
 }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-         accountNumber:String,
- balance:Double,
- accountType:String
-        }
-</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -112,21 +99,6 @@
   </si>
   <si>
     <t>Admin Approval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{userId:Long,
-firstName:String,
-lastName:String,
-address:String,
-age:Int
-purpose:String,
-email:String,
-city:String,
-phNum:Long,
-gender:String,
-accountType:String,status:String
-}
-</t>
   </si>
   <si>
     <t>/api/approval/{userId}</t>
@@ -289,9 +261,21 @@
 </t>
   </si>
   <si>
-    <t>{
+    <t>{loginId:String,
+ password:String,
+ mortgageNumber:String,
+accountNumber:String,
 message:String
 }</t>
+  </si>
+  <si>
+    <t>{
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{message:String
+}
+</t>
   </si>
 </sst>
 </file>
@@ -741,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -775,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>2</v>
@@ -789,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -803,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -815,7 +799,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -827,10 +811,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -839,10 +823,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -851,13 +835,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -865,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -879,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -893,13 +877,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -907,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -937,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
@@ -951,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -965,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -977,10 +961,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -989,10 +973,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1001,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -1013,7 +997,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -1025,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1037,10 +1021,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1049,7 +1033,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
@@ -1061,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -1073,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
@@ -1085,7 +1069,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -1097,10 +1081,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1109,7 +1093,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -1133,13 +1117,13 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1147,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>2</v>
@@ -1161,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>4</v>
@@ -1175,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>18</v>
@@ -1187,7 +1171,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -1199,10 +1183,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D40" s="1"/>
     </row>
@@ -1211,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1223,13 +1207,13 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1248,8 +1232,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1279,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>11</v>
@@ -1299,41 +1283,41 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="165.75">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="38.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -1343,60 +1327,56 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="76.5">
+    <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="165.75">
+    <row r="7" spans="1:8">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Data Contract Updates commited By 'Lakshmi'
</commit_message>
<xml_diff>
--- a/Mortgage_Data_Contract.xlsx
+++ b/Mortgage_Data_Contract.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -85,25 +85,6 @@
     <t>varchar</t>
   </si>
   <si>
-    <t>{
-userId: Long,password: String
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-         accountNumber:String,
- balance:Double,
- accountType:String,userId:Long
-        }
-</t>
-  </si>
-  <si>
-    <t>Admin Approval</t>
-  </si>
-  <si>
-    <t>/api/approval/{userId}</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -230,13 +211,7 @@
     <t>AccountSummary</t>
   </si>
   <si>
-    <t>/api/accountSummary</t>
-  </si>
-  <si>
     <t>Transaction Details</t>
-  </si>
-  <si>
-    <t>/api/transactions</t>
   </si>
   <si>
     <t xml:space="preserve">URL                                                                    Request Contract </t>
@@ -276,6 +251,30 @@
     <t xml:space="preserve">{message:String
 }
 </t>
+  </si>
+  <si>
+    <t>{
+}</t>
+  </si>
+  <si>
+    <t>/api/accountSummary/{customerId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ accountNumber:String,
+ balance:Double,
+ accountType:String
+        }
+</t>
+  </si>
+  <si>
+    <t>/api/transactions/{accountNumber}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{amount:Double,traansactionDate;Date,transactionTime:Time}</t>
   </si>
 </sst>
 </file>
@@ -725,7 +724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>2</v>
@@ -773,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -787,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -799,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -811,10 +810,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -823,10 +822,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -835,13 +834,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -849,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -863,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -877,13 +876,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -891,7 +890,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -921,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
@@ -935,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -949,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -961,10 +960,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -973,10 +972,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -985,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -997,7 +996,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -1009,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1021,10 +1020,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1033,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
@@ -1045,7 +1044,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -1057,7 +1056,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
@@ -1069,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -1081,10 +1080,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1093,7 +1092,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -1117,13 +1116,13 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1131,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>2</v>
@@ -1145,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>4</v>
@@ -1159,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>18</v>
@@ -1171,7 +1170,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -1183,10 +1182,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D40" s="1"/>
     </row>
@@ -1195,10 +1194,10 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1207,13 +1206,13 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1232,15 +1231,15 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="45.625" customWidth="1"/>
     <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
@@ -1263,7 +1262,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>11</v>
@@ -1283,19 +1282,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1305,19 +1304,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -1327,19 +1326,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1349,16 +1348,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
@@ -1366,15 +1369,9 @@
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="1"/>

</xml_diff>

<commit_message>
Batch Processing  Api  commited By 'Lakshmi'
</commit_message>
<xml_diff>
--- a/Mortgage_Data_Contract.xlsx
+++ b/Mortgage_Data_Contract.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -275,6 +275,18 @@
   </si>
   <si>
     <t>{amount:Double,traansactionDate;Date,transactionTime:Time}</t>
+  </si>
+  <si>
+    <t>Batch Process</t>
+  </si>
+  <si>
+    <t>/api/batchUpdate</t>
+  </si>
+  <si>
+    <t>{message:String}</t>
+  </si>
+  <si>
+    <t>DrOrCr</t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,6 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -390,6 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,7 +736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,10 +747,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A2:D42"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -748,22 +760,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -844,16 +856,16 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -916,16 +928,16 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1028,114 +1040,114 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="2">
+      <c r="A27" s="12">
         <v>9</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="2"/>
+      <c r="C27" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="12"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2">
+      <c r="A28" s="12">
         <v>10</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2"/>
+      <c r="C28" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="12"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="2">
+      <c r="A29" s="12">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2"/>
+      <c r="C29" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="2">
+      <c r="A30" s="12">
         <v>12</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2"/>
+      <c r="C30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="2">
+      <c r="A31" s="12">
         <v>13</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="2">
+      <c r="A32" s="12">
         <v>14</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="C32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="2">
+      <c r="A33" s="12">
         <v>15</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2"/>
+      <c r="C33" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="2">
+      <c r="A34" s="12">
         <v>16</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1206,12 +1218,24 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1231,8 +1255,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1246,206 +1270,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="216.75">
-      <c r="A3" s="6">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="216.75">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="38.25">
-      <c r="A4" s="6">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="38.25">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="76.5">
-      <c r="A5" s="6">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="76.5">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1">
-      <c r="A6" s="6">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>

</xml_diff>